<commit_message>
Changed default property value locations
Removed methods inside of units to get move range, etc. Instead, all
units have a UnitStat object that points to their classes' default
UnitStat in the DefaultStats class.
</commit_message>
<xml_diff>
--- a/resources/unitstatstest.xlsx
+++ b/resources/unitstatstest.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Unit_Name</t>
   </si>
@@ -22,10 +22,10 @@
     <t>Armor</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>Range</t>
+    <t>Ability_Power</t>
+  </si>
+  <si>
+    <t>Ability_Range</t>
   </si>
   <si>
     <t>Side_Block(OCOH)</t>
@@ -34,7 +34,10 @@
     <t>Front_Block(OCOH)</t>
   </si>
   <si>
-    <t>Movement</t>
+    <t>Can_Move</t>
+  </si>
+  <si>
+    <t>Move_Range</t>
   </si>
   <si>
     <t>Wait</t>
@@ -251,10 +254,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>50.0</v>
@@ -274,16 +280,19 @@
       <c r="G2" s="2">
         <v>0.2</v>
       </c>
-      <c r="H2" s="1">
-        <v>3.0</v>
+      <c r="H2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J2" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>50.0</v>
@@ -303,16 +312,19 @@
       <c r="G3" s="2">
         <v>0.1</v>
       </c>
-      <c r="H3" s="1">
-        <v>3.0</v>
+      <c r="H3" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I3" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J3" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>30.0</v>
@@ -332,16 +344,19 @@
       <c r="G4" s="2">
         <v>0.4</v>
       </c>
-      <c r="H4" s="1">
-        <v>3.0</v>
+      <c r="H4" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J4" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>28.0</v>
@@ -361,16 +376,19 @@
       <c r="G5" s="2">
         <v>0.3</v>
       </c>
-      <c r="H5" s="1">
-        <v>4.0</v>
+      <c r="H5" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J5" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>35.0</v>
@@ -390,16 +408,19 @@
       <c r="G6" s="2">
         <v>0.0</v>
       </c>
-      <c r="H6" s="1">
-        <v>3.0</v>
+      <c r="H6" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I6" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J6" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>40.0</v>
@@ -419,16 +440,19 @@
       <c r="G7" s="2">
         <v>0.4</v>
       </c>
-      <c r="H7" s="1">
-        <v>4.0</v>
+      <c r="H7" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J7" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>35.0</v>
@@ -448,16 +472,19 @@
       <c r="G8" s="2">
         <v>0.3</v>
       </c>
-      <c r="H8" s="1">
-        <v>3.0</v>
+      <c r="H8" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I8" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J8" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>40.0</v>
@@ -477,16 +504,19 @@
       <c r="G9" s="2">
         <v>0.5</v>
       </c>
-      <c r="H9" s="1">
-        <v>3.0</v>
+      <c r="H9" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I9" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J9" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
         <v>28.0</v>
@@ -506,16 +536,19 @@
       <c r="G10" s="2">
         <v>0.9</v>
       </c>
-      <c r="H10" s="1">
-        <v>3.0</v>
+      <c r="H10" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I10" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J10" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>28.0</v>
@@ -535,16 +568,19 @@
       <c r="G11" s="2">
         <v>0.9</v>
       </c>
-      <c r="H11" s="1">
-        <v>3.0</v>
+      <c r="H11" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I11" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J11" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>24.0</v>
@@ -556,7 +592,7 @@
         <v>12.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2">
         <v>0.0</v>
@@ -564,16 +600,19 @@
       <c r="G12" s="2">
         <v>0.0</v>
       </c>
-      <c r="H12" s="1">
-        <v>4.0</v>
+      <c r="H12" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I12" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J12" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>18.0</v>
@@ -585,7 +624,7 @@
         <v>22.0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2">
         <v>0.0</v>
@@ -593,16 +632,19 @@
       <c r="G13" s="2">
         <v>0.0</v>
       </c>
-      <c r="H13" s="1">
-        <v>3.0</v>
+      <c r="H13" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I13" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J13" s="1">
         <v>7.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>35.0</v>
@@ -622,16 +664,19 @@
       <c r="G14" s="2">
         <v>0.1</v>
       </c>
-      <c r="H14" s="1">
-        <v>4.0</v>
+      <c r="H14" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I14" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J14" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>35.0</v>
@@ -643,7 +688,7 @@
         <v>18.0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" s="2">
         <v>0.7</v>
@@ -651,16 +696,19 @@
       <c r="G15" s="2">
         <v>0.4</v>
       </c>
-      <c r="H15" s="1">
-        <v>4.0</v>
+      <c r="H15" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I15" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J15" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1">
         <v>30.0</v>
@@ -672,7 +720,7 @@
         <v>21.0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="2">
         <v>0.45</v>
@@ -680,16 +728,19 @@
       <c r="G16" s="2">
         <v>0.3</v>
       </c>
-      <c r="H16" s="1">
-        <v>4.0</v>
+      <c r="H16" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I16" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J16" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>30.0</v>
@@ -698,7 +749,7 @@
         <v>0.0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" s="1">
         <v>3.0</v>
@@ -709,16 +760,19 @@
       <c r="G17" s="2">
         <v>0.0</v>
       </c>
-      <c r="H17" s="1">
-        <v>3.0</v>
+      <c r="H17" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I17" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J17" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>35.0</v>
@@ -727,7 +781,7 @@
         <v>0.0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1">
         <v>0.0</v>
@@ -738,16 +792,19 @@
       <c r="G18" s="2">
         <v>0.0</v>
       </c>
-      <c r="H18" s="1">
-        <v>4.0</v>
+      <c r="H18" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I18" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J18" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>32.0</v>
@@ -756,7 +813,7 @@
         <v>0.0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1">
         <v>6.0</v>
@@ -767,16 +824,19 @@
       <c r="G19" s="2">
         <v>1.0</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="H19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>56.0</v>
@@ -796,16 +856,19 @@
       <c r="G20" s="2">
         <v>1.0</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="H20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1">
         <v>50.0</v>
@@ -814,7 +877,7 @@
         <v>12.0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1">
         <v>3.0</v>
@@ -825,16 +888,19 @@
       <c r="G21" s="2">
         <v>1.0</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="H21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1">
         <v>38.0</v>
@@ -854,16 +920,19 @@
       <c r="G22" s="2">
         <v>0.2</v>
       </c>
-      <c r="H22" s="1">
-        <v>4.0</v>
+      <c r="H22" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I22" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J22" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>52.0</v>
@@ -883,16 +952,19 @@
       <c r="G23" s="2">
         <v>0.3</v>
       </c>
-      <c r="H23" s="1">
-        <v>3.0</v>
+      <c r="H23" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I23" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J23" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>38.0</v>
@@ -912,16 +984,19 @@
       <c r="G24" s="2">
         <v>0.5</v>
       </c>
-      <c r="H24" s="1">
-        <v>4.0</v>
+      <c r="H24" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I24" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J24" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1">
         <v>48.0</v>
@@ -930,7 +1005,7 @@
         <v>0.0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E25" s="1">
         <v>2.0</v>
@@ -941,16 +1016,19 @@
       <c r="G25" s="2">
         <v>0.2</v>
       </c>
-      <c r="H25" s="1">
-        <v>4.0</v>
+      <c r="H25" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I25" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J25" s="1">
         <v>1.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1">
         <v>48.0</v>
@@ -959,7 +1037,7 @@
         <v>0.0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E26" s="1">
         <v>3.0</v>
@@ -970,16 +1048,19 @@
       <c r="G26" s="2">
         <v>0.2</v>
       </c>
-      <c r="H26" s="1">
-        <v>3.0</v>
+      <c r="H26" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I26" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J26" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>34.0</v>
@@ -991,7 +1072,7 @@
         <v>4.0</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F27" s="2">
         <v>0.0</v>
@@ -999,16 +1080,19 @@
       <c r="G27" s="2">
         <v>0.0</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
         <v>6.0</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>68.0</v>
@@ -1020,7 +1104,7 @@
         <v>28.0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F28" s="2">
         <v>0.6</v>
@@ -1028,16 +1112,19 @@
       <c r="G28" s="2">
         <v>0.4</v>
       </c>
-      <c r="H28" s="1">
-        <v>4.0</v>
+      <c r="H28" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I28" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J28" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1">
         <v>60.0</v>
@@ -1054,16 +1141,19 @@
       <c r="F29" s="2">
         <v>0.3</v>
       </c>
-      <c r="H29" s="1">
-        <v>3.0</v>
+      <c r="H29" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I29" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J29" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1">
         <v>60.0</v>
@@ -1080,22 +1170,25 @@
       <c r="F30" s="2">
         <v>0.5</v>
       </c>
-      <c r="H30" s="1">
-        <v>4.0</v>
+      <c r="H30" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I30" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J30" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1">
         <v>60.0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>20.0</v>
@@ -1109,22 +1202,25 @@
       <c r="G31" s="2">
         <v>0.0</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
         <v>5.0</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1">
         <v>60.0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1">
         <v>20.0</v>
@@ -1138,22 +1234,25 @@
       <c r="G32" s="2">
         <v>0.0</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
         <v>2.0</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>3.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" s="1">
         <v>60.0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1">
         <v>20.0</v>
@@ -1167,22 +1266,25 @@
       <c r="G33" s="2">
         <v>0.0</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
         <v>5.0</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B34" s="1">
         <v>60.0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D34" s="1">
         <v>20.0</v>
@@ -1196,16 +1298,19 @@
       <c r="G34" s="2">
         <v>0.0</v>
       </c>
-      <c r="H34" s="1">
-        <v>4.0</v>
+      <c r="H34" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I34" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J34" s="1">
         <v>2.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1">
         <v>60.0</v>
@@ -1214,27 +1319,30 @@
         <v>30.0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E35" s="1">
         <v>1.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G35" s="2">
         <v>0.0</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
         <v>2.0</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>4.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B36" s="1">
         <v>60.0</v>
@@ -1243,50 +1351,56 @@
         <v>30.0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E36" s="1">
         <v>1.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G36" s="2">
         <v>0.0</v>
       </c>
-      <c r="H36" s="1">
-        <v>1.0</v>
+      <c r="H36" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="I36" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J36" s="1">
         <v>6.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B37" s="1">
         <v>60.0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E37" s="1">
         <v>1.0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G37" s="2">
         <v>0.0</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
         <v>5.0</v>
       </c>
-      <c r="I37" s="1">
+      <c r="J37" s="1">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>